<commit_message>
Create Excel file and work with Background Colors
</commit_message>
<xml_diff>
--- a/airtravel.xlsx
+++ b/airtravel.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Raw data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -26,12 +26,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00aa5624"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <gradientFill type="linear">
+        <stop position="0">
+          <color rgb="00FFFFFF"/>
+        </stop>
+        <stop position="1">
+          <color rgb="00000000"/>
+        </stop>
+      </gradientFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +61,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,7 +443,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Month</t>
         </is>
@@ -437,7 +458,7 @@
           <t xml:space="preserve"> "1959"</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> "1960"</t>
         </is>

</xml_diff>

<commit_message>
Update headers functions to place headers with format in a vertical or a horizontal format in the Excel file
</commit_message>
<xml_diff>
--- a/airtravel.xlsx
+++ b/airtravel.xlsx
@@ -26,6 +26,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
       <b val="1"/>
       <sz val="12"/>
     </font>
@@ -38,12 +39,6 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="007CAAF0"/>
-        <bgColor rgb="007CAAF0"/>
-      </patternFill>
-    </fill>
-    <fill>
       <gradientFill type="linear">
         <stop position="0">
           <color rgb="00FFFFFF"/>
@@ -52,6 +47,12 @@
           <color rgb="00000000"/>
         </stop>
       </gradientFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="007CAAF0"/>
+        <bgColor rgb="007CAAF0"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,12 +69,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -439,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,7 +451,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Month</t>
         </is>
@@ -476,7 +473,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>JAN</t>
         </is>
@@ -498,7 +495,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>FEB</t>
         </is>
@@ -520,7 +517,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>MAR</t>
         </is>
@@ -547,7 +544,7 @@
           <t>APR</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">  348</t>
         </is>
@@ -564,7 +561,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -586,7 +583,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>JUN</t>
         </is>
@@ -608,7 +605,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>JUL</t>
         </is>
@@ -630,7 +627,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>AUG</t>
         </is>
@@ -652,7 +649,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>SEP</t>
         </is>
@@ -674,7 +671,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>OCT</t>
         </is>
@@ -696,7 +693,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>NOV</t>
         </is>
@@ -718,7 +715,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>DEC</t>
         </is>
@@ -739,7 +736,6 @@
         </is>
       </c>
     </row>
-    <row r="14"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
New files with data in horizontal
</commit_message>
<xml_diff>
--- a/airtravel.xlsx
+++ b/airtravel.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Raw data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Horizontal_Data" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -739,4 +740,130 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="81.59999999999999" customWidth="1" min="1" max="1"/>
+    <col width="7.199999999999999" customWidth="1" min="2" max="2"/>
+    <col width="7.199999999999999" customWidth="1" min="3" max="3"/>
+    <col width="7.199999999999999" customWidth="1" min="4" max="4"/>
+    <col width="7.199999999999999" customWidth="1" min="5" max="5"/>
+    <col width="7.199999999999999" customWidth="1" min="6" max="6"/>
+    <col width="7.199999999999999" customWidth="1" min="7" max="7"/>
+    <col width="7.199999999999999" customWidth="1" min="8" max="8"/>
+    <col width="7.199999999999999" customWidth="1" min="9" max="9"/>
+    <col width="7.199999999999999" customWidth="1" min="10" max="10"/>
+    <col width="7.199999999999999" customWidth="1" min="11" max="11"/>
+    <col width="7.199999999999999" customWidth="1" min="12" max="12"/>
+    <col width="7.199999999999999" customWidth="1" min="13" max="13"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Month</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> JAN</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> FEB</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MAR</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> APR</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MAY</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> JUN</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> JUL</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> AUG</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SEP</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> OCT</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> NOV</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> DEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>"1958", 340, 318, 362, 348, 363, 435, 491, 505, 404, 359, 310, 337</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>"1959", 360, 342, 406, 396, 420, 472, 548, 559, 463, 407, 362, 405</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>"1960", 417, 391, 419, 461, 472, 535, 622, 606, 508, 461, 390, 432</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n"/>
+      <c r="B5" s="1" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Function to adapt the style of headers cells depending of orientation of the table in the worksheet
</commit_message>
<xml_diff>
--- a/airtravel.xlsx
+++ b/airtravel.xlsx
@@ -443,7 +443,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="8.4" customWidth="1" min="1" max="1"/>
     <col width="10.8" customWidth="1" min="2" max="2"/>
@@ -754,9 +754,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="81.59999999999999" customWidth="1" min="1" max="1"/>
+    <col width="8.4" customWidth="1" min="1" max="1"/>
     <col width="7.199999999999999" customWidth="1" min="2" max="2"/>
     <col width="7.199999999999999" customWidth="1" min="3" max="3"/>
     <col width="7.199999999999999" customWidth="1" min="4" max="4"/>
@@ -777,90 +777,269 @@
           <t>Month</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> JAN</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> FEB</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> MAR</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> APR</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> MAY</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> JUN</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> JUL</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> AUG</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> SEP</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> OCT</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> NOV</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> DEC</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>"1958", 340, 318, 362, 348, 363, 435, 491, 505, 404, 359, 310, 337</t>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1958</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 340</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 318</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 362</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 348</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 363</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 435</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 491</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 505</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 404</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 359</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 310</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 337</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>"1959", 360, 342, 406, 396, 420, 472, 548, 559, 463, 407, 362, 405</t>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1959</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 360</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 342</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 406</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 396</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 420</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 472</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 548</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 559</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 463</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 407</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 362</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 405</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>"1960", 417, 391, 419, 461, 472, 535, 622, 606, 508, 461, 390, 432</t>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 417</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 391</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 419</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 461</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 472</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 535</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 622</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 606</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 508</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 461</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 390</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 432</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n"/>
       <c r="B5" s="1" t="n"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Draft version of code for line_charts
</commit_message>
<xml_diff>
--- a/airtravel.xlsx
+++ b/airtravel.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Raw data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rawdata" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Horizontal_Data" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
@@ -146,6 +146,151 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Sales per month</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Rawdata'!B7</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Rawdata'!$B$1:$D$1</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Rawdata'!$B$8:$B$13</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Month</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Ticket Sales (USD Mil)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="b"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,7 +588,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8.4" customWidth="1" min="1" max="1"/>
     <col width="10.8" customWidth="1" min="2" max="2"/>
@@ -739,6 +884,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -754,7 +900,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="8.4" customWidth="1" min="1" max="1"/>
     <col width="7.199999999999999" customWidth="1" min="2" max="2"/>
@@ -777,69 +923,69 @@
           <t>Month</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t xml:space="preserve"> JAN</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t xml:space="preserve"> FEB</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t xml:space="preserve"> MAR</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t xml:space="preserve"> APR</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t xml:space="preserve"> MAY</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t xml:space="preserve"> JUN</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t xml:space="preserve"> JUL</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t xml:space="preserve"> AUG</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t xml:space="preserve"> SEP</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t xml:space="preserve"> OCT</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t xml:space="preserve"> NOV</t>
         </is>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t xml:space="preserve"> DEC</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>1958</t>
         </is>
@@ -906,7 +1052,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>1959</t>
         </is>
@@ -973,7 +1119,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>1960</t>
         </is>
@@ -1040,6 +1186,7 @@
       </c>
     </row>
     <row r="5">
+      <c r="A5" s="2" t="n"/>
       <c r="B5" s="1" t="n"/>
     </row>
   </sheetData>

</xml_diff>